<commit_message>
Added PatternSizeEvaluations and some results
</commit_message>
<xml_diff>
--- a/results/resultsOverview.xlsx
+++ b/results/resultsOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\eclipse-workspaces\re.actionEvaluation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98991F52-00F2-489D-BBEC-E99B1C363532}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4AC0F2-BB73-4C2D-8BA3-9BDA1406E649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30768AEB-27FD-4976-8FEF-D014ED9BAB80}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
   <si>
     <t>Specs:</t>
   </si>
@@ -122,6 +122,12 @@
   <si>
     <t>16 GB DDR3 RAM</t>
   </si>
+  <si>
+    <t>Pattern Size Variation (1000 Iterations)</t>
+  </si>
+  <si>
+    <t>Mustergröße</t>
+  </si>
 </sst>
 </file>
 
@@ -177,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -265,48 +271,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -321,10 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1660,7 +1625,7 @@
                   <c:v>1286.9597475</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16741.375866499999</c:v>
+                  <c:v>11289.7171225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,6 +1696,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1404.4564593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14090.156771800001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2209,7 +2177,7 @@
                   <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11020</c:v>
+                  <c:v>13424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,6 +2248,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2928,7 +2899,7 @@
                   <c:v>1342</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11020</c:v>
+                  <c:v>13424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3007,6 +2978,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3661,7 +3635,7 @@
                   <c:v>298.85119300000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16741.375866499999</c:v>
+                  <c:v>11289.7171225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3734,6 +3708,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>331.57160770000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14090.156771800001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3924,6 +3901,1138 @@
                 <a:r>
                   <a:rPr lang="de-DE" baseline="0"/>
                   <a:t> [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419744568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Laufzeit Pattern Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>"HiPE Bidirektional"</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$35,Tabelle1!$F$35,Tabelle1!$G$35,Tabelle1!$H$35,Tabelle1!$I$35)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.6077591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3935616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4067217999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>202.786967</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FD0D-4E61-B06D-3D9A67079BCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Democles Bidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$37,Tabelle1!$F$37,Tabelle1!$G$37,Tabelle1!$H$37,Tabelle1!$I$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.38508890000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7352841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4939206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.170130700000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FD0D-4E61-B06D-3D9A67079BCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>HiPE Unidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$41,Tabelle1!$F$41,Tabelle1!$G$41,Tabelle1!$H$41,Tabelle1!$I$41)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-FD0D-4E61-B06D-3D9A67079BCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Democles Unidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$43,Tabelle1!$F$43,Tabelle1!$G$43,Tabelle1!$H$43,Tabelle1!$I$43)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-FD0D-4E61-B06D-3D9A67079BCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="419744568"/>
+        <c:axId val="419739648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="419744568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>#Parameter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419739648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="419739648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Laufzeit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419744568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Speicherverbrauch Pattern Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>HiPE Bidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$36,Tabelle1!$F$36,Tabelle1!$G$36,Tabelle1!$H$36,Tabelle1!$I$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-670C-4AA3-87C9-1455F3DDDD32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Democles Bidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$38,Tabelle1!$F$38,Tabelle1!$G$38,Tabelle1!$H$38,Tabelle1!$I$38)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6409</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-670C-4AA3-87C9-1455F3DDDD32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>HiPE Unidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$42,Tabelle1!$F$42,Tabelle1!$G$42,Tabelle1!$H$42,Tabelle1!$I$42)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-670C-4AA3-87C9-1455F3DDDD32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Democles Unidirektional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$E$44,Tabelle1!$F$44,Tabelle1!$G$44,Tabelle1!$H$44,Tabelle1!$I$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-670C-4AA3-87C9-1455F3DDDD32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="419744568"/>
+        <c:axId val="419739648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="419744568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>#Parameter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419739648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="419739648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Speicherverbrauch</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [MB]</a:t>
                 </a:r>
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
@@ -4316,6 +5425,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6897,6 +8086,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7640,6 +9861,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>728382</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>296428</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>62161</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagramm 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19D5355A-9D14-4E50-890A-3035A23F8F71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>526676</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>783099</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Diagramm 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CD1EC-5F92-4431-A7F5-4833D4A12E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7940,10 +10237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63F4900-11DB-40C4-900A-4EEDCE9D26ED}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7963,7 +10260,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="25" t="s">
         <v>15</v>
       </c>
     </row>
@@ -8036,10 +10333,10 @@
       <c r="I5" s="3">
         <v>1286.9597475</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="14">
-        <v>16741.375866499999</v>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4">
+        <v>11289.7171225</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -8061,10 +10358,10 @@
       <c r="I6" s="6">
         <v>2048</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="15">
-        <v>11020</v>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="7">
+        <v>13424</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -8088,9 +10385,11 @@
       <c r="I7" s="9">
         <v>1404.4564593</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="16"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10">
+        <v>14090.156771800001</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -8111,9 +10410,11 @@
       <c r="I8" s="12">
         <v>1985</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="17"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13">
+        <v>10528</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
@@ -8184,13 +10485,13 @@
       <c r="I11" s="3">
         <v>1250.0942887000001</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>2431.4618473999999</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>3665.2150136999999</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="4">
         <v>9992.9143846000006</v>
       </c>
     </row>
@@ -8215,13 +10516,13 @@
       <c r="I12" s="6">
         <v>2340</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>5977</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>5291</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="7">
         <v>10535</v>
       </c>
     </row>
@@ -8248,11 +10549,11 @@
       <c r="I13" s="9">
         <v>1382.7936012</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>2510.7646770000001</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="16">
+      <c r="K13" s="9"/>
+      <c r="L13" s="10">
         <v>19764.4232672</v>
       </c>
     </row>
@@ -8277,11 +10578,11 @@
       <c r="I14" s="12">
         <v>2697</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <v>5487</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="17">
+      <c r="K14" s="12"/>
+      <c r="L14" s="13">
         <v>10442</v>
       </c>
     </row>
@@ -8321,7 +10622,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="18">
+      <c r="C23" s="14">
         <v>0.2</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -8342,62 +10643,292 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="17">
         <v>1031</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="17">
         <v>1835</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="17">
         <v>1763</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="18">
         <v>3187</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="23">
+      <c r="C25" s="19">
         <v>0.4</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="19"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="28" t="s">
+      <c r="H26" s="24" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>40</v>
+      </c>
+      <c r="F33" s="1">
+        <v>60</v>
+      </c>
+      <c r="G33" s="1">
+        <v>80</v>
+      </c>
+      <c r="H33" s="1">
+        <v>100</v>
+      </c>
+      <c r="I33" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>4</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5</v>
+      </c>
+      <c r="I34" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.6077591</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1.3935616</v>
+      </c>
+      <c r="G35" s="3">
+        <v>9.4067217999999997</v>
+      </c>
+      <c r="H35" s="3">
+        <v>202.786967</v>
+      </c>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="6">
+        <v>113</v>
+      </c>
+      <c r="F36" s="6">
+        <v>138</v>
+      </c>
+      <c r="G36" s="6">
+        <v>561</v>
+      </c>
+      <c r="H36" s="6">
+        <v>4295</v>
+      </c>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0.38508890000000001</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0.7352841</v>
+      </c>
+      <c r="G37" s="9">
+        <v>3.4939206</v>
+      </c>
+      <c r="H37" s="9">
+        <v>50.170130700000001</v>
+      </c>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="12">
+        <v>68</v>
+      </c>
+      <c r="F38" s="12">
+        <v>116</v>
+      </c>
+      <c r="G38" s="12">
+        <v>904</v>
+      </c>
+      <c r="H38" s="12">
+        <v>6409</v>
+      </c>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>40</v>
+      </c>
+      <c r="F39" s="1">
+        <v>60</v>
+      </c>
+      <c r="G39" s="1">
+        <v>80</v>
+      </c>
+      <c r="H39" s="1">
+        <v>100</v>
+      </c>
+      <c r="I39" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3</v>
+      </c>
+      <c r="G40" s="1">
+        <v>4</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5</v>
+      </c>
+      <c r="I40" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>